<commit_message>
moved scripts from src to imbalance and added test cases for split_data
</commit_message>
<xml_diff>
--- a/imbalance_model_metrics.xlsx
+++ b/imbalance_model_metrics.xlsx
@@ -631,21 +631,21 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[[32814 24043]
- [    8    97]]</t>
+          <t>[[56819    38]
+ [   24    81]]</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.5777711456760647</v>
+        <v>0.9989115550718023</v>
       </c>
       <c r="G4" t="n">
-        <v>0.004018227009113504</v>
+        <v>0.680672268907563</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9238095238095239</v>
+        <v>0.7714285714285715</v>
       </c>
       <c r="I4" t="n">
-        <v>0.008001649824706124</v>
+        <v>0.7232142857142857</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -654,15 +654,15 @@
         <v>12978.07</v>
       </c>
       <c r="L4" t="n">
-        <v>471158.39</v>
+        <v>3194.11</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>3630.4195462037114%</t>
+          <t>24.611594790288542%</t>
         </is>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -686,21 +686,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[[26447 19046]
- [    8    68]]</t>
+          <t>[[45464    29]
+ [   19    57]]</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.5818648642717636</v>
+        <v>0.9989466523294345</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00355760175787381</v>
+        <v>0.6627906976744186</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8947368421052632</v>
+        <v>0.75</v>
       </c>
       <c r="I5" t="n">
-        <v>0.007087024491922876</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -709,15 +709,15 @@
         <v>7031.66</v>
       </c>
       <c r="L5" t="n">
-        <v>273638.3</v>
+        <v>272.23</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>3891.517792384728%</t>
+          <t>3.8714898046833897%</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -851,21 +851,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[[ 2863 53994]
- [    1   104]]</t>
+          <t>[[55163  1694]
+ [   17    88]]</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.05208735648326955</v>
+        <v>0.9699624310944138</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0019224370586713</v>
+        <v>0.04938271604938271</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9904761904761905</v>
+        <v>0.8380952380952381</v>
       </c>
       <c r="I8" t="n">
-        <v>0.003837425972732137</v>
+        <v>0.09326974032856386</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -874,15 +874,15 @@
         <v>12978.07</v>
       </c>
       <c r="L8" t="n">
-        <v>1024110.19</v>
+        <v>31273.06</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>7891.08234121098%</t>
+          <t>240.96849531555927%</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -906,21 +906,21 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[[ 2397 43096]
- [    0    76]]</t>
+          <t>[[44267  1226]
+ [   12    64]]</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.05426934977726085</v>
+        <v>0.9728324079966644</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001760400259427407</v>
+        <v>0.04961240310077519</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="I9" t="n">
-        <v>0.003514613392526822</v>
+        <v>0.09370424597364568</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
@@ -929,15 +929,15 @@
         <v>7031.66</v>
       </c>
       <c r="L9" t="n">
-        <v>628056.71</v>
+        <v>16635.83</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>8931.841272188927%</t>
+          <t>236.5846755958053%</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">

</xml_diff>